<commit_message>
Made in 1b_child_counts_and_census.qmd chi-square and corrplot() ready tables for national racial representations. Yay 🥳
</commit_message>
<xml_diff>
--- a/Data/racial group representation in general population and in EI NATIONAL.xlsx
+++ b/Data/racial group representation in general population and in EI NATIONAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Desktop/EDLD652_Diss/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B4B57E-A932-E541-BA22-585B5E5E4E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6F8B70-4D39-6F42-B06F-96934D2395EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10860" yWindow="9160" windowWidth="18560" windowHeight="15920" xr2:uid="{5BDF04D4-4642-B244-951B-A64689ECD2CF}"/>
+    <workbookView xWindow="9780" yWindow="500" windowWidth="21200" windowHeight="15980" xr2:uid="{5BDF04D4-4642-B244-951B-A64689ECD2CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.7598872019938241E-2"/>
+          <c:y val="0.11586140808645254"/>
+          <c:w val="0.94240112798006181"/>
+          <c:h val="0.79326829380931485"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1512,16 +1522,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>736600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1868,7 +1878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16AB9D85-4B21-8B41-AC42-E6E9EED8B3CD}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>